<commit_message>
Updated password service tests
</commit_message>
<xml_diff>
--- a/iddd_identityaccess/java_test_list..xlsx
+++ b/iddd_identityaccess/java_test_list..xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
   <si>
     <t>AccessApplicationServiceTest.java</t>
   </si>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1348,6 +1348,9 @@
       <c r="B67" t="s">
         <v>75</v>
       </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
@@ -1356,6 +1359,9 @@
       <c r="B68" t="s">
         <v>76</v>
       </c>
+      <c r="D68" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
@@ -1364,6 +1370,9 @@
       <c r="B69" t="s">
         <v>77</v>
       </c>
+      <c r="D69" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
@@ -1372,6 +1381,9 @@
       <c r="B70" t="s">
         <v>78</v>
       </c>
+      <c r="D70" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
@@ -1447,6 +1459,9 @@
       <c r="B79" t="s">
         <v>67</v>
       </c>
+      <c r="D79" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
@@ -1455,6 +1470,9 @@
       <c r="B80" t="s">
         <v>89</v>
       </c>
+      <c r="D80" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
@@ -1463,6 +1481,9 @@
       <c r="B81" t="s">
         <v>69</v>
       </c>
+      <c r="D81" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
@@ -1471,6 +1492,9 @@
       <c r="B82" t="s">
         <v>90</v>
       </c>
+      <c r="D82" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
@@ -1703,11 +1727,11 @@
     <row r="107" spans="1:5">
       <c r="D107">
         <f>COUNTIF(D2:D106, "Y")</f>
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E107">
         <f>D107/ROWS(B2:B106)</f>
-        <v>0.25714285714285712</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to stuff
</commit_message>
<xml_diff>
--- a/iddd_identityaccess/java_test_list..xlsx
+++ b/iddd_identityaccess/java_test_list..xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="java_test_list.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="123">
   <si>
     <t>AccessApplicationServiceTest.java</t>
   </si>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1028,6 +1028,9 @@
       <c r="B24" t="s">
         <v>25</v>
       </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
@@ -1036,6 +1039,9 @@
       <c r="B25" t="s">
         <v>26</v>
       </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
@@ -1044,6 +1050,9 @@
       <c r="B26" t="s">
         <v>27</v>
       </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
@@ -1800,6 +1809,9 @@
       <c r="B95" t="s">
         <v>105</v>
       </c>
+      <c r="D95" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
@@ -1840,6 +1852,9 @@
       <c r="B100" t="s">
         <v>112</v>
       </c>
+      <c r="D100" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
@@ -1848,6 +1863,9 @@
       <c r="B101" t="s">
         <v>114</v>
       </c>
+      <c r="D101" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
@@ -1856,6 +1874,9 @@
       <c r="B102" t="s">
         <v>115</v>
       </c>
+      <c r="D102" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
@@ -1864,6 +1885,9 @@
       <c r="B103" t="s">
         <v>116</v>
       </c>
+      <c r="D103" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
@@ -1872,6 +1896,9 @@
       <c r="B104" t="s">
         <v>117</v>
       </c>
+      <c r="D104" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
@@ -1880,6 +1907,9 @@
       <c r="B105" t="s">
         <v>2</v>
       </c>
+      <c r="D105" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
@@ -1888,15 +1918,18 @@
       <c r="B106" t="s">
         <v>118</v>
       </c>
+      <c r="D106" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="107" spans="1:5">
       <c r="D107">
         <f>COUNTIF(D2:D106, "Y")</f>
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E107">
         <f>D107/ROWS(B2:B106)</f>
-        <v>0.8571428571428571</v>
+        <v>0.96190476190476193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>